<commit_message>
[FIX] clean code and Calculated new formula
</commit_message>
<xml_diff>
--- a/eco_project_report/report_project/report_project.xlsx
+++ b/eco_project_report/report_project/report_project.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t xml:space="preserve">Support Summary</t>
   </si>
@@ -60,28 +60,34 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">Duration Time (Hours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effective (Hours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used Man-Hour Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spent Time (Hours)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used Man-Hour Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finished</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject</t>
   </si>
 </sst>
 </file>
@@ -286,7 +292,7 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -388,7 +394,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -397,8 +403,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -409,6 +415,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
@@ -432,6 +439,9 @@
       </c>
       <c r="E3" s="7" t="s">
         <v>12</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="ALR3" s="0"/>
       <c r="ALS3" s="0"/>
@@ -455,7 +465,7 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:E2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -492,7 +502,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -512,25 +522,25 @@
     </row>
     <row r="3" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="ALT3" s="0"/>
       <c r="ALU3" s="0"/>

</xml_diff>

<commit_message>
[FIX] report and add used time in support
</commit_message>
<xml_diff>
--- a/eco_project_report/report_project/report_project.xlsx
+++ b/eco_project_report/report_project/report_project.xlsx
@@ -5,12 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Support Package" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Used Man-Hour" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Used Time" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,32 +21,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t xml:space="preserve">Support Summary</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Support Ticket</t>
+    <t xml:space="preserve">Support Time (Not Expiry)</t>
   </si>
   <si>
     <t xml:space="preserve">Hour(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Task Close</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Used Man-Hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Task In-Progress</t>
+    <t xml:space="preserve">Used Time (Not Expiry)</t>
   </si>
   <si>
     <t xml:space="preserve">Balance</t>
   </si>
   <si>
-    <t xml:space="preserve">Support Package Description</t>
-  </si>
-  <si>
     <t xml:space="preserve">Start Date</t>
   </si>
   <si>
@@ -63,7 +53,7 @@
     <t xml:space="preserve">Duration Time (Hours)</t>
   </si>
   <si>
-    <t xml:space="preserve">Effective (Hours)</t>
+    <t xml:space="preserve">Used Time (Hours)</t>
   </si>
   <si>
     <t xml:space="preserve">Used Man-Hour Description</t>
@@ -88,6 +78,9 @@
   </si>
   <si>
     <t xml:space="preserve">Spent Time (Hours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package Name</t>
   </si>
 </sst>
 </file>
@@ -176,7 +169,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -197,16 +190,24 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -290,18 +291,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
@@ -334,42 +336,59 @@
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>2</v>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -394,57 +413,69 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="ALR3" s="0"/>
-      <c r="ALS3" s="0"/>
+      <c r="C3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="ALT3" s="0"/>
       <c r="ALU3" s="0"/>
       <c r="ALV3" s="0"/>
@@ -465,105 +496,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:E2"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AMJ3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="ALT3" s="0"/>
-      <c r="ALU3" s="0"/>
-      <c r="ALV3" s="0"/>
-      <c r="ALW3" s="0"/>
-      <c r="ALX3" s="0"/>
-      <c r="ALY3" s="0"/>
-      <c r="ALZ3" s="0"/>
-      <c r="AMA3" s="0"/>
-      <c r="AMB3" s="0"/>
-      <c r="AMC3" s="0"/>
-      <c r="AMD3" s="0"/>
-      <c r="AME3" s="0"/>
-      <c r="AMF3" s="0"/>
-      <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
[ENH] project support ecosoft to v.2
</commit_message>
<xml_diff>
--- a/eco_project_report/report_project/report_project.xlsx
+++ b/eco_project_report/report_project/report_project.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Used Time" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="In-Progress" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,18 +22,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t xml:space="preserve">Support Summary</t>
   </si>
   <si>
-    <t xml:space="preserve">Support Time (Not Expiry)</t>
+    <t xml:space="preserve">Duration Time</t>
   </si>
   <si>
     <t xml:space="preserve">Hour(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Used Time (Not Expiry)</t>
+    <t xml:space="preserve">Used Time</t>
   </si>
   <si>
     <t xml:space="preserve">Balance</t>
@@ -81,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">Package Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Progress</t>
   </si>
 </sst>
 </file>
@@ -135,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -143,6 +147,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -169,7 +180,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,6 +223,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -293,7 +308,7 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -414,7 +429,7 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -507,4 +522,55 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>